<commit_message>
Small edits on existing plots and new boxplot
</commit_message>
<xml_diff>
--- a/HEATMAP.xlsx
+++ b/HEATMAP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynreahl/Documents/BergmannLab_2018-2020/Reahl_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F063890-7127-7D4B-B8D1-A4A1A308AA67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C4B877-A472-9145-88FC-C0140A00FF44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="440" windowWidth="12300" windowHeight="14180" xr2:uid="{75335D1A-4D0E-7A45-9BB4-AFE682FEF120}"/>
+    <workbookView xWindow="4060" yWindow="440" windowWidth="18340" windowHeight="14180" activeTab="3" xr2:uid="{75335D1A-4D0E-7A45-9BB4-AFE682FEF120}"/>
   </bookViews>
   <sheets>
     <sheet name="MODERN" sheetId="4" r:id="rId1"/>
@@ -634,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF51893-7E80-8548-B6F8-7BC70CFF8579}">
   <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -9998,10 +9998,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBEB359-EE0E-5B4D-87E8-356B5BEC7DF0}">
-  <dimension ref="A1:AP28"/>
+  <dimension ref="A1:AQ28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10009,7 +10009,7 @@
     <col min="3" max="42" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -10077,7 +10077,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>32</v>
       </c>
@@ -10085,67 +10085,87 @@
         <v>30</v>
       </c>
       <c r="C2" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.20512820512820512</v>
       </c>
       <c r="D2" s="4">
-        <v>0.2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>0.65</v>
+        <v>0.46153846153846151</v>
       </c>
       <c r="F2" s="4">
-        <v>0.4</v>
+        <v>0.38461538461538469</v>
       </c>
       <c r="G2" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>5.128205128205128E-2</v>
       </c>
       <c r="H2" s="4">
-        <v>0.15</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="I2" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.23076923076923075</v>
       </c>
       <c r="J2" s="4">
-        <v>0.9</v>
+        <v>0.48717948717948717</v>
       </c>
       <c r="K2" s="4">
         <v>1</v>
       </c>
       <c r="L2" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.12820512820512819</v>
       </c>
       <c r="M2" s="4">
-        <v>0.2</v>
+        <v>0.20512820512820512</v>
       </c>
       <c r="N2" s="4">
         <v>1</v>
       </c>
       <c r="O2" s="4">
-        <v>0.45</v>
+        <v>0.17948717948717949</v>
       </c>
       <c r="P2" s="4">
-        <v>7.4999999999999997E-2</v>
+        <v>0.12820512820512819</v>
       </c>
       <c r="Q2" s="4">
-        <v>0.125</v>
+        <v>0.17948717948717949</v>
       </c>
       <c r="R2" s="4">
-        <v>0.85</v>
+        <v>0.97435897435897434</v>
       </c>
       <c r="S2" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0.15</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0.64102564102564097</v>
+      </c>
+      <c r="U2" s="4">
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="V2" s="4">
+        <v>2.564102564102564E-2</v>
+      </c>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>33</v>
       </c>
@@ -10153,67 +10173,67 @@
         <v>30</v>
       </c>
       <c r="C3" s="4">
-        <v>0.20512820512820512</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D3" s="4">
-        <v>7.6923076923076927E-2</v>
+        <v>0.2</v>
       </c>
       <c r="E3" s="4">
-        <v>0.46153846153846151</v>
+        <v>0.65</v>
       </c>
       <c r="F3" s="4">
-        <v>0.38461538461538469</v>
+        <v>0.4</v>
       </c>
       <c r="G3" s="4">
-        <v>5.128205128205128E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H3" s="4">
-        <v>0.15384615384615385</v>
+        <v>0.15</v>
       </c>
       <c r="I3" s="4">
-        <v>0.23076923076923075</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J3" s="4">
-        <v>0.48717948717948717</v>
+        <v>0.9</v>
       </c>
       <c r="K3" s="4">
         <v>1</v>
       </c>
       <c r="L3" s="4">
-        <v>0.12820512820512819</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M3" s="4">
-        <v>0.20512820512820512</v>
+        <v>0.2</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
       </c>
       <c r="O3" s="4">
-        <v>0.17948717948717949</v>
+        <v>0.45</v>
       </c>
       <c r="P3" s="4">
-        <v>0.12820512820512819</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="Q3" s="4">
-        <v>0.17948717948717949</v>
+        <v>0.125</v>
       </c>
       <c r="R3" s="4">
-        <v>0.97435897435897434</v>
+        <v>0.85</v>
       </c>
       <c r="S3" s="4">
-        <v>1</v>
-      </c>
-      <c r="T3" s="4">
-        <v>0.64102564102564097</v>
-      </c>
-      <c r="U3" s="4">
-        <v>0.33333333333333326</v>
-      </c>
-      <c r="V3" s="4">
-        <v>2.564102564102564E-2</v>
+        <v>0.7</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>34</v>
       </c>
@@ -10281,7 +10301,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>35</v>
       </c>
@@ -10349,7 +10369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -10417,7 +10437,7 @@
         <v>0.177978</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>45</v>
       </c>
@@ -10485,7 +10505,7 @@
         <v>9.5454545454545597E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>46</v>
       </c>
@@ -10553,7 +10573,7 @@
         <v>7.2727272727272696E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>47</v>
       </c>
@@ -10621,7 +10641,7 @@
         <v>4.9999999999999906E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>48</v>
       </c>
@@ -10709,7 +10729,7 @@
       <c r="AO10" s="3"/>
       <c r="AP10" s="3"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>49</v>
       </c>
@@ -10777,7 +10797,7 @@
         <v>0.18210116730000001</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -10865,7 +10885,7 @@
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>36</v>
       </c>
@@ -10953,7 +10973,7 @@
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>37</v>
       </c>
@@ -11041,7 +11061,7 @@
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>38</v>
       </c>
@@ -11129,7 +11149,7 @@
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>39</v>
       </c>

</xml_diff>